<commit_message>
update data-raw and inst-data
</commit_message>
<xml_diff>
--- a/inst/extdata/zooplankton/Arzp20.xlsx
+++ b/inst/extdata/zooplankton/Arzp20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evanamies-galonski/Code/nrp/nrp/inst/extdata/zooplankton/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3485D45B-9978-2D41-ACC5-DFBDA2C7984E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CFF339-9B85-BD40-BFC9-AD015838162E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="31720" windowHeight="19680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -546,9 +546,6 @@
     <t>Month</t>
   </si>
   <si>
-    <t>Date1</t>
-  </si>
-  <si>
     <t>Date2</t>
   </si>
   <si>
@@ -793,6 +790,9 @@
   </si>
   <si>
     <t>FieldCollection</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -1207,10 +1207,10 @@
   <dimension ref="A1:FO105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="EM2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="FO13" sqref="FO13"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1237,22 +1237,22 @@
         <v>170</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="G1" t="s">
         <v>171</v>
-      </c>
-      <c r="G1" t="s">
-        <v>172</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>174</v>
       </c>
       <c r="K1" t="s">
         <v>2</v>
@@ -1273,7 +1273,7 @@
         <v>7</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="R1" t="s">
         <v>8</v>
@@ -1393,7 +1393,7 @@
         <v>46</v>
       </c>
       <c r="BE1" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="BF1" t="s">
         <v>47</v>
@@ -1720,22 +1720,22 @@
         <v>154</v>
       </c>
       <c r="FJ1" t="s">
+        <v>176</v>
+      </c>
+      <c r="FK1" t="s">
         <v>177</v>
       </c>
-      <c r="FK1" t="s">
+      <c r="FL1" t="s">
+        <v>251</v>
+      </c>
+      <c r="FM1" t="s">
+        <v>252</v>
+      </c>
+      <c r="FN1" t="s">
         <v>178</v>
       </c>
-      <c r="FL1" t="s">
-        <v>252</v>
-      </c>
-      <c r="FM1" t="s">
-        <v>253</v>
-      </c>
-      <c r="FN1" t="s">
-        <v>179</v>
-      </c>
       <c r="FO1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:171" x14ac:dyDescent="0.2">
@@ -1749,10 +1749,10 @@
         <v>2020</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F2" s="7">
         <v>43941</v>
@@ -1764,10 +1764,10 @@
         <v>1</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="K2" s="1">
         <v>1</v>
@@ -2225,13 +2225,13 @@
         <v>1</v>
       </c>
       <c r="FL2" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM2" t="s">
         <v>249</v>
       </c>
-      <c r="FM2" t="s">
+      <c r="FN2" t="s">
         <v>250</v>
-      </c>
-      <c r="FN2" t="s">
-        <v>251</v>
       </c>
       <c r="FO2" s="1">
         <v>100</v>
@@ -2248,10 +2248,10 @@
         <v>2020</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F3" s="7">
         <v>43941</v>
@@ -2263,10 +2263,10 @@
         <v>2</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="K3" s="1">
         <v>1</v>
@@ -2724,13 +2724,13 @@
         <v>2</v>
       </c>
       <c r="FL3" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM3" t="s">
         <v>249</v>
       </c>
-      <c r="FM3" t="s">
+      <c r="FN3" t="s">
         <v>250</v>
-      </c>
-      <c r="FN3" t="s">
-        <v>251</v>
       </c>
       <c r="FO3" s="1">
         <v>100</v>
@@ -2747,10 +2747,10 @@
         <v>2020</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F4" s="7">
         <v>43941</v>
@@ -2762,10 +2762,10 @@
         <v>3</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="K4" s="1">
         <v>1</v>
@@ -3223,13 +3223,13 @@
         <v>1</v>
       </c>
       <c r="FL4" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM4" t="s">
         <v>249</v>
       </c>
-      <c r="FM4" t="s">
+      <c r="FN4" t="s">
         <v>250</v>
-      </c>
-      <c r="FN4" t="s">
-        <v>251</v>
       </c>
       <c r="FO4" s="1">
         <v>100</v>
@@ -3246,10 +3246,10 @@
         <v>2020</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F5" s="7">
         <v>43943</v>
@@ -3261,10 +3261,10 @@
         <v>6</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K5" s="1">
         <v>1</v>
@@ -3722,13 +3722,13 @@
         <v>1</v>
       </c>
       <c r="FL5" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM5" t="s">
         <v>249</v>
       </c>
-      <c r="FM5" t="s">
+      <c r="FN5" t="s">
         <v>250</v>
-      </c>
-      <c r="FN5" t="s">
-        <v>251</v>
       </c>
       <c r="FO5" s="1">
         <v>100</v>
@@ -3745,10 +3745,10 @@
         <v>2020</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F6" s="7">
         <v>43943</v>
@@ -3760,10 +3760,10 @@
         <v>7</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K6" s="1">
         <v>1</v>
@@ -4221,13 +4221,13 @@
         <v>2</v>
       </c>
       <c r="FL6" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM6" t="s">
         <v>249</v>
       </c>
-      <c r="FM6" t="s">
+      <c r="FN6" t="s">
         <v>250</v>
-      </c>
-      <c r="FN6" t="s">
-        <v>251</v>
       </c>
       <c r="FO6" s="1">
         <v>100</v>
@@ -4244,10 +4244,10 @@
         <v>2020</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F7" s="7">
         <v>43943</v>
@@ -4259,10 +4259,10 @@
         <v>8</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K7" s="1">
         <v>1</v>
@@ -4720,13 +4720,13 @@
         <v>1</v>
       </c>
       <c r="FL7" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM7" t="s">
         <v>249</v>
       </c>
-      <c r="FM7" t="s">
+      <c r="FN7" t="s">
         <v>250</v>
-      </c>
-      <c r="FN7" t="s">
-        <v>251</v>
       </c>
       <c r="FO7" s="1">
         <v>100</v>
@@ -4743,10 +4743,10 @@
         <v>2020</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F8" s="7">
         <v>43941</v>
@@ -4758,10 +4758,10 @@
         <v>1</v>
       </c>
       <c r="I8" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="K8" s="1">
         <v>2</v>
@@ -5219,13 +5219,13 @@
         <v>2</v>
       </c>
       <c r="FL8" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM8" t="s">
         <v>249</v>
       </c>
-      <c r="FM8" t="s">
+      <c r="FN8" t="s">
         <v>250</v>
-      </c>
-      <c r="FN8" t="s">
-        <v>251</v>
       </c>
       <c r="FO8" s="1">
         <v>100</v>
@@ -5242,10 +5242,10 @@
         <v>2020</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F9" s="7">
         <v>43941</v>
@@ -5257,10 +5257,10 @@
         <v>2</v>
       </c>
       <c r="I9" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="K9" s="1">
         <v>2</v>
@@ -5718,13 +5718,13 @@
         <v>2</v>
       </c>
       <c r="FL9" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM9" t="s">
         <v>249</v>
       </c>
-      <c r="FM9" t="s">
+      <c r="FN9" t="s">
         <v>250</v>
-      </c>
-      <c r="FN9" t="s">
-        <v>251</v>
       </c>
       <c r="FO9" s="1">
         <v>100</v>
@@ -5741,10 +5741,10 @@
         <v>2020</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F10" s="7">
         <v>43941</v>
@@ -5756,10 +5756,10 @@
         <v>3</v>
       </c>
       <c r="I10" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="K10" s="1">
         <v>2</v>
@@ -6217,13 +6217,13 @@
         <v>2</v>
       </c>
       <c r="FL10" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM10" t="s">
         <v>249</v>
       </c>
-      <c r="FM10" t="s">
+      <c r="FN10" t="s">
         <v>250</v>
-      </c>
-      <c r="FN10" t="s">
-        <v>251</v>
       </c>
       <c r="FO10" s="1">
         <v>100</v>
@@ -6240,10 +6240,10 @@
         <v>2020</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F11" s="7">
         <v>43943</v>
@@ -6255,10 +6255,10 @@
         <v>6</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K11" s="1">
         <v>2</v>
@@ -6716,13 +6716,13 @@
         <v>1</v>
       </c>
       <c r="FL11" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM11" t="s">
         <v>249</v>
       </c>
-      <c r="FM11" t="s">
+      <c r="FN11" t="s">
         <v>250</v>
-      </c>
-      <c r="FN11" t="s">
-        <v>251</v>
       </c>
       <c r="FO11" s="1">
         <v>100</v>
@@ -6739,10 +6739,10 @@
         <v>2020</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F12" s="7">
         <v>43943</v>
@@ -6754,10 +6754,10 @@
         <v>7</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K12" s="1">
         <v>2</v>
@@ -7215,13 +7215,13 @@
         <v>2</v>
       </c>
       <c r="FL12" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM12" t="s">
         <v>249</v>
       </c>
-      <c r="FM12" t="s">
+      <c r="FN12" t="s">
         <v>250</v>
-      </c>
-      <c r="FN12" t="s">
-        <v>251</v>
       </c>
       <c r="FO12" s="1">
         <v>100</v>
@@ -7238,10 +7238,10 @@
         <v>2020</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F13" s="7">
         <v>43943</v>
@@ -7253,10 +7253,10 @@
         <v>8</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K13" s="1">
         <v>2</v>
@@ -7714,13 +7714,13 @@
         <v>2</v>
       </c>
       <c r="FL13" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM13" t="s">
         <v>249</v>
       </c>
-      <c r="FM13" t="s">
+      <c r="FN13" t="s">
         <v>250</v>
-      </c>
-      <c r="FN13" t="s">
-        <v>251</v>
       </c>
       <c r="FO13" s="1">
         <v>100</v>
@@ -7740,7 +7740,7 @@
     </row>
     <row r="15" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B15" s="3">
         <v>2020</v>
@@ -7749,10 +7749,10 @@
         <v>2020</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F15" s="9">
         <v>43969</v>
@@ -7764,10 +7764,10 @@
         <v>2</v>
       </c>
       <c r="I15" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J15" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -8229,13 +8229,13 @@
         <v>2</v>
       </c>
       <c r="FL15" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM15" t="s">
         <v>249</v>
       </c>
-      <c r="FM15" t="s">
+      <c r="FN15" t="s">
         <v>250</v>
-      </c>
-      <c r="FN15" t="s">
-        <v>251</v>
       </c>
       <c r="FO15" s="1">
         <v>100</v>
@@ -8243,7 +8243,7 @@
     </row>
     <row r="16" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B16" s="3">
         <v>2020</v>
@@ -8252,10 +8252,10 @@
         <v>2020</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F16" s="9">
         <v>43969</v>
@@ -8267,10 +8267,10 @@
         <v>3</v>
       </c>
       <c r="I16" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J16" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -8732,13 +8732,13 @@
         <v>1</v>
       </c>
       <c r="FL16" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM16" t="s">
         <v>249</v>
       </c>
-      <c r="FM16" t="s">
+      <c r="FN16" t="s">
         <v>250</v>
-      </c>
-      <c r="FN16" t="s">
-        <v>251</v>
       </c>
       <c r="FO16" s="1">
         <v>100</v>
@@ -8758,7 +8758,7 @@
     </row>
     <row r="18" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B18" s="3">
         <v>2020</v>
@@ -8767,10 +8767,10 @@
         <v>2020</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F18" s="9">
         <v>43969</v>
@@ -8782,10 +8782,10 @@
         <v>7</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -9247,13 +9247,13 @@
         <v>2</v>
       </c>
       <c r="FL18" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM18" t="s">
         <v>249</v>
       </c>
-      <c r="FM18" t="s">
+      <c r="FN18" t="s">
         <v>250</v>
-      </c>
-      <c r="FN18" t="s">
-        <v>251</v>
       </c>
       <c r="FO18" s="1">
         <v>100</v>
@@ -9261,7 +9261,7 @@
     </row>
     <row r="19" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B19" s="3">
         <v>2020</v>
@@ -9270,10 +9270,10 @@
         <v>2020</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F19" s="9">
         <v>43969</v>
@@ -9285,10 +9285,10 @@
         <v>8</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -9750,13 +9750,13 @@
         <v>2</v>
       </c>
       <c r="FL19" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM19" t="s">
         <v>249</v>
       </c>
-      <c r="FM19" t="s">
+      <c r="FN19" t="s">
         <v>250</v>
-      </c>
-      <c r="FN19" t="s">
-        <v>251</v>
       </c>
       <c r="FO19" s="1">
         <v>100</v>
@@ -9776,7 +9776,7 @@
     </row>
     <row r="21" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B21" s="3">
         <v>2020</v>
@@ -9785,10 +9785,10 @@
         <v>2020</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F21" s="9">
         <v>43969</v>
@@ -9800,10 +9800,10 @@
         <v>2</v>
       </c>
       <c r="I21" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J21" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="K21">
         <v>2</v>
@@ -10265,13 +10265,13 @@
         <v>1</v>
       </c>
       <c r="FL21" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM21" t="s">
         <v>249</v>
       </c>
-      <c r="FM21" t="s">
+      <c r="FN21" t="s">
         <v>250</v>
-      </c>
-      <c r="FN21" t="s">
-        <v>251</v>
       </c>
       <c r="FO21" s="1">
         <v>100</v>
@@ -10279,7 +10279,7 @@
     </row>
     <row r="22" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B22" s="3">
         <v>2020</v>
@@ -10288,10 +10288,10 @@
         <v>2020</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F22" s="9">
         <v>43969</v>
@@ -10303,10 +10303,10 @@
         <v>3</v>
       </c>
       <c r="I22" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J22" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="K22">
         <v>2</v>
@@ -10768,13 +10768,13 @@
         <v>2</v>
       </c>
       <c r="FL22" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM22" t="s">
         <v>249</v>
       </c>
-      <c r="FM22" t="s">
+      <c r="FN22" t="s">
         <v>250</v>
-      </c>
-      <c r="FN22" t="s">
-        <v>251</v>
       </c>
       <c r="FO22" s="1">
         <v>100</v>
@@ -10794,7 +10794,7 @@
     </row>
     <row r="24" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B24" s="3">
         <v>2020</v>
@@ -10803,10 +10803,10 @@
         <v>2020</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F24" s="9">
         <v>43969</v>
@@ -10818,10 +10818,10 @@
         <v>7</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K24">
         <v>2</v>
@@ -11283,13 +11283,13 @@
         <v>2</v>
       </c>
       <c r="FL24" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM24" t="s">
         <v>249</v>
       </c>
-      <c r="FM24" t="s">
+      <c r="FN24" t="s">
         <v>250</v>
-      </c>
-      <c r="FN24" t="s">
-        <v>251</v>
       </c>
       <c r="FO24" s="1">
         <v>100</v>
@@ -11297,7 +11297,7 @@
     </row>
     <row r="25" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B25" s="3">
         <v>2020</v>
@@ -11306,10 +11306,10 @@
         <v>2020</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F25" s="9">
         <v>43969</v>
@@ -11321,10 +11321,10 @@
         <v>8</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K25">
         <v>2</v>
@@ -11786,13 +11786,13 @@
         <v>2</v>
       </c>
       <c r="FL25" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM25" t="s">
         <v>249</v>
       </c>
-      <c r="FM25" t="s">
+      <c r="FN25" t="s">
         <v>250</v>
-      </c>
-      <c r="FN25" t="s">
-        <v>251</v>
       </c>
       <c r="FO25" s="1">
         <v>100</v>
@@ -11813,7 +11813,7 @@
     </row>
     <row r="27" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B27" s="3">
         <v>2020</v>
@@ -11822,10 +11822,10 @@
         <v>2020</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F27" s="9">
         <v>43997</v>
@@ -11837,10 +11837,10 @@
         <v>2</v>
       </c>
       <c r="I27" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J27" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -12302,13 +12302,13 @@
         <v>2</v>
       </c>
       <c r="FL27" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM27" t="s">
         <v>249</v>
       </c>
-      <c r="FM27" t="s">
+      <c r="FN27" t="s">
         <v>250</v>
-      </c>
-      <c r="FN27" t="s">
-        <v>251</v>
       </c>
       <c r="FO27" s="1">
         <v>100</v>
@@ -12316,7 +12316,7 @@
     </row>
     <row r="28" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B28" s="3">
         <v>2020</v>
@@ -12325,10 +12325,10 @@
         <v>2020</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F28" s="9">
         <v>43997</v>
@@ -12340,10 +12340,10 @@
         <v>3</v>
       </c>
       <c r="I28" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J28" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="K28">
         <v>1</v>
@@ -12805,13 +12805,13 @@
         <v>2</v>
       </c>
       <c r="FL28" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM28" t="s">
         <v>249</v>
       </c>
-      <c r="FM28" t="s">
+      <c r="FN28" t="s">
         <v>250</v>
-      </c>
-      <c r="FN28" t="s">
-        <v>251</v>
       </c>
       <c r="FO28" s="1">
         <v>100</v>
@@ -12832,7 +12832,7 @@
     </row>
     <row r="30" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B30" s="3">
         <v>2020</v>
@@ -12841,10 +12841,10 @@
         <v>2020</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F30" s="9">
         <v>43997</v>
@@ -12856,10 +12856,10 @@
         <v>7</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K30">
         <v>1</v>
@@ -13321,13 +13321,13 @@
         <v>2</v>
       </c>
       <c r="FL30" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM30" t="s">
         <v>249</v>
       </c>
-      <c r="FM30" t="s">
+      <c r="FN30" t="s">
         <v>250</v>
-      </c>
-      <c r="FN30" t="s">
-        <v>251</v>
       </c>
       <c r="FO30" s="1">
         <v>100</v>
@@ -13335,7 +13335,7 @@
     </row>
     <row r="31" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B31" s="3">
         <v>2020</v>
@@ -13344,10 +13344,10 @@
         <v>2020</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F31" s="9">
         <v>43997</v>
@@ -13359,10 +13359,10 @@
         <v>8</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K31">
         <v>1</v>
@@ -13824,13 +13824,13 @@
         <v>1</v>
       </c>
       <c r="FL31" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM31" t="s">
         <v>249</v>
       </c>
-      <c r="FM31" t="s">
+      <c r="FN31" t="s">
         <v>250</v>
-      </c>
-      <c r="FN31" t="s">
-        <v>251</v>
       </c>
       <c r="FO31" s="1">
         <v>100</v>
@@ -13851,7 +13851,7 @@
     </row>
     <row r="33" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B33" s="3">
         <v>2020</v>
@@ -13860,10 +13860,10 @@
         <v>2020</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F33" s="9">
         <v>43997</v>
@@ -13875,10 +13875,10 @@
         <v>2</v>
       </c>
       <c r="I33" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J33" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="K33">
         <v>2</v>
@@ -14340,13 +14340,13 @@
         <v>1</v>
       </c>
       <c r="FL33" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM33" t="s">
         <v>249</v>
       </c>
-      <c r="FM33" t="s">
+      <c r="FN33" t="s">
         <v>250</v>
-      </c>
-      <c r="FN33" t="s">
-        <v>251</v>
       </c>
       <c r="FO33" s="1">
         <v>100</v>
@@ -14354,7 +14354,7 @@
     </row>
     <row r="34" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B34" s="3">
         <v>2020</v>
@@ -14363,10 +14363,10 @@
         <v>2020</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F34" s="9">
         <v>43997</v>
@@ -14378,10 +14378,10 @@
         <v>3</v>
       </c>
       <c r="I34" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J34" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="K34">
         <v>2</v>
@@ -14843,13 +14843,13 @@
         <v>2</v>
       </c>
       <c r="FL34" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM34" t="s">
         <v>249</v>
       </c>
-      <c r="FM34" t="s">
+      <c r="FN34" t="s">
         <v>250</v>
-      </c>
-      <c r="FN34" t="s">
-        <v>251</v>
       </c>
       <c r="FO34" s="1">
         <v>100</v>
@@ -14870,7 +14870,7 @@
     </row>
     <row r="36" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B36" s="3">
         <v>2020</v>
@@ -14879,10 +14879,10 @@
         <v>2020</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F36" s="9">
         <v>43997</v>
@@ -14894,10 +14894,10 @@
         <v>7</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K36">
         <v>2</v>
@@ -15359,13 +15359,13 @@
         <v>1</v>
       </c>
       <c r="FL36" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM36" t="s">
         <v>249</v>
       </c>
-      <c r="FM36" t="s">
+      <c r="FN36" t="s">
         <v>250</v>
-      </c>
-      <c r="FN36" t="s">
-        <v>251</v>
       </c>
       <c r="FO36" s="1">
         <v>100</v>
@@ -15373,7 +15373,7 @@
     </row>
     <row r="37" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B37" s="3">
         <v>2020</v>
@@ -15382,10 +15382,10 @@
         <v>2020</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F37" s="9">
         <v>43997</v>
@@ -15397,10 +15397,10 @@
         <v>8</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K37">
         <v>2</v>
@@ -15862,13 +15862,13 @@
         <v>2</v>
       </c>
       <c r="FL37" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM37" t="s">
         <v>249</v>
       </c>
-      <c r="FM37" t="s">
+      <c r="FN37" t="s">
         <v>250</v>
-      </c>
-      <c r="FN37" t="s">
-        <v>251</v>
       </c>
       <c r="FO37" s="1">
         <v>100</v>
@@ -15888,7 +15888,7 @@
     </row>
     <row r="39" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B39" s="3">
         <v>2020</v>
@@ -15897,10 +15897,10 @@
         <v>2020</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F39" s="9">
         <v>44025</v>
@@ -15912,10 +15912,10 @@
         <v>2</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K39">
         <v>1</v>
@@ -16377,13 +16377,13 @@
         <v>2</v>
       </c>
       <c r="FL39" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM39" t="s">
         <v>249</v>
       </c>
-      <c r="FM39" t="s">
+      <c r="FN39" t="s">
         <v>250</v>
-      </c>
-      <c r="FN39" t="s">
-        <v>251</v>
       </c>
       <c r="FO39" s="1">
         <v>100</v>
@@ -16391,7 +16391,7 @@
     </row>
     <row r="40" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B40" s="3">
         <v>2020</v>
@@ -16400,10 +16400,10 @@
         <v>2020</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F40" s="9">
         <v>44025</v>
@@ -16415,10 +16415,10 @@
         <v>3</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K40">
         <v>1</v>
@@ -16880,13 +16880,13 @@
         <v>2</v>
       </c>
       <c r="FL40" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM40" t="s">
         <v>249</v>
       </c>
-      <c r="FM40" t="s">
+      <c r="FN40" t="s">
         <v>250</v>
-      </c>
-      <c r="FN40" t="s">
-        <v>251</v>
       </c>
       <c r="FO40" s="1">
         <v>100</v>
@@ -16906,7 +16906,7 @@
     </row>
     <row r="42" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B42" s="3">
         <v>2020</v>
@@ -16915,10 +16915,10 @@
         <v>2020</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F42" s="9">
         <v>44025</v>
@@ -16930,10 +16930,10 @@
         <v>7</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K42">
         <v>1</v>
@@ -17395,13 +17395,13 @@
         <v>1</v>
       </c>
       <c r="FL42" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM42" t="s">
         <v>249</v>
       </c>
-      <c r="FM42" t="s">
+      <c r="FN42" t="s">
         <v>250</v>
-      </c>
-      <c r="FN42" t="s">
-        <v>251</v>
       </c>
       <c r="FO42" s="1">
         <v>100</v>
@@ -17409,7 +17409,7 @@
     </row>
     <row r="43" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B43" s="3">
         <v>2020</v>
@@ -17418,10 +17418,10 @@
         <v>2020</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F43" s="9">
         <v>44025</v>
@@ -17433,10 +17433,10 @@
         <v>8</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K43">
         <v>1</v>
@@ -17898,13 +17898,13 @@
         <v>1</v>
       </c>
       <c r="FL43" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM43" t="s">
         <v>249</v>
       </c>
-      <c r="FM43" t="s">
+      <c r="FN43" t="s">
         <v>250</v>
-      </c>
-      <c r="FN43" t="s">
-        <v>251</v>
       </c>
       <c r="FO43" s="1">
         <v>100</v>
@@ -17924,7 +17924,7 @@
     </row>
     <row r="45" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B45" s="3">
         <v>2020</v>
@@ -17933,10 +17933,10 @@
         <v>2020</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F45" s="9">
         <v>44025</v>
@@ -17948,10 +17948,10 @@
         <v>2</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K45">
         <v>2</v>
@@ -18413,13 +18413,13 @@
         <v>1</v>
       </c>
       <c r="FL45" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM45" t="s">
         <v>249</v>
       </c>
-      <c r="FM45" t="s">
+      <c r="FN45" t="s">
         <v>250</v>
-      </c>
-      <c r="FN45" t="s">
-        <v>251</v>
       </c>
       <c r="FO45" s="1">
         <v>100</v>
@@ -18427,7 +18427,7 @@
     </row>
     <row r="46" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B46" s="3">
         <v>2020</v>
@@ -18436,10 +18436,10 @@
         <v>2020</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F46" s="9">
         <v>44025</v>
@@ -18451,10 +18451,10 @@
         <v>3</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K46">
         <v>1</v>
@@ -18916,13 +18916,13 @@
         <v>2</v>
       </c>
       <c r="FL46" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM46" t="s">
         <v>249</v>
       </c>
-      <c r="FM46" t="s">
+      <c r="FN46" t="s">
         <v>250</v>
-      </c>
-      <c r="FN46" t="s">
-        <v>251</v>
       </c>
       <c r="FO46" s="1">
         <v>100</v>
@@ -18942,7 +18942,7 @@
     </row>
     <row r="48" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B48" s="3">
         <v>2020</v>
@@ -18951,10 +18951,10 @@
         <v>2020</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F48" s="9">
         <v>44025</v>
@@ -18966,10 +18966,10 @@
         <v>7</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K48">
         <v>2</v>
@@ -19431,13 +19431,13 @@
         <v>1</v>
       </c>
       <c r="FL48" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM48" t="s">
         <v>249</v>
       </c>
-      <c r="FM48" t="s">
+      <c r="FN48" t="s">
         <v>250</v>
-      </c>
-      <c r="FN48" t="s">
-        <v>251</v>
       </c>
       <c r="FO48" s="1">
         <v>100</v>
@@ -19445,7 +19445,7 @@
     </row>
     <row r="49" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B49" s="3">
         <v>2020</v>
@@ -19454,10 +19454,10 @@
         <v>2020</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F49" s="9">
         <v>44025</v>
@@ -19469,10 +19469,10 @@
         <v>8</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K49">
         <v>2</v>
@@ -19934,13 +19934,13 @@
         <v>1</v>
       </c>
       <c r="FL49" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM49" t="s">
         <v>249</v>
       </c>
-      <c r="FM49" t="s">
+      <c r="FN49" t="s">
         <v>250</v>
-      </c>
-      <c r="FN49" t="s">
-        <v>251</v>
       </c>
       <c r="FO49" s="1">
         <v>100</v>
@@ -19962,7 +19962,7 @@
     </row>
     <row r="51" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B51" s="3">
         <v>2020</v>
@@ -19971,10 +19971,10 @@
         <v>2020</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F51" s="9">
         <v>44053</v>
@@ -19986,10 +19986,10 @@
         <v>2</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K51">
         <v>1</v>
@@ -20451,13 +20451,13 @@
         <v>1</v>
       </c>
       <c r="FL51" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM51" t="s">
         <v>249</v>
       </c>
-      <c r="FM51" t="s">
+      <c r="FN51" t="s">
         <v>250</v>
-      </c>
-      <c r="FN51" t="s">
-        <v>251</v>
       </c>
       <c r="FO51" s="1">
         <v>100</v>
@@ -20465,7 +20465,7 @@
     </row>
     <row r="52" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B52" s="3">
         <v>2020</v>
@@ -20474,10 +20474,10 @@
         <v>2020</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F52" s="9">
         <v>44053</v>
@@ -20489,10 +20489,10 @@
         <v>3</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K52">
         <v>1</v>
@@ -20954,13 +20954,13 @@
         <v>1</v>
       </c>
       <c r="FL52" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM52" t="s">
         <v>249</v>
       </c>
-      <c r="FM52" t="s">
+      <c r="FN52" t="s">
         <v>250</v>
-      </c>
-      <c r="FN52" t="s">
-        <v>251</v>
       </c>
       <c r="FO52" s="1">
         <v>100</v>
@@ -20980,7 +20980,7 @@
     </row>
     <row r="54" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B54" s="3">
         <v>2020</v>
@@ -20989,10 +20989,10 @@
         <v>2020</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F54" s="9">
         <v>44053</v>
@@ -21004,10 +21004,10 @@
         <v>7</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K54">
         <v>1</v>
@@ -21469,13 +21469,13 @@
         <v>1</v>
       </c>
       <c r="FL54" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM54" t="s">
         <v>249</v>
       </c>
-      <c r="FM54" t="s">
+      <c r="FN54" t="s">
         <v>250</v>
-      </c>
-      <c r="FN54" t="s">
-        <v>251</v>
       </c>
       <c r="FO54" s="1">
         <v>100</v>
@@ -21483,7 +21483,7 @@
     </row>
     <row r="55" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B55" s="3">
         <v>2020</v>
@@ -21492,10 +21492,10 @@
         <v>2020</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F55" s="9">
         <v>44053</v>
@@ -21507,10 +21507,10 @@
         <v>8</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K55">
         <v>1</v>
@@ -21972,13 +21972,13 @@
         <v>2</v>
       </c>
       <c r="FL55" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM55" t="s">
         <v>249</v>
       </c>
-      <c r="FM55" t="s">
+      <c r="FN55" t="s">
         <v>250</v>
-      </c>
-      <c r="FN55" t="s">
-        <v>251</v>
       </c>
       <c r="FO55" s="1">
         <v>100</v>
@@ -21998,7 +21998,7 @@
     </row>
     <row r="57" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B57" s="3">
         <v>2020</v>
@@ -22007,10 +22007,10 @@
         <v>2020</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F57" s="9">
         <v>44053</v>
@@ -22022,10 +22022,10 @@
         <v>2</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K57">
         <v>2</v>
@@ -22487,13 +22487,13 @@
         <v>1</v>
       </c>
       <c r="FL57" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM57" t="s">
         <v>249</v>
       </c>
-      <c r="FM57" t="s">
+      <c r="FN57" t="s">
         <v>250</v>
-      </c>
-      <c r="FN57" t="s">
-        <v>251</v>
       </c>
       <c r="FO57" s="1">
         <v>100</v>
@@ -22501,7 +22501,7 @@
     </row>
     <row r="58" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B58" s="3">
         <v>2020</v>
@@ -22510,10 +22510,10 @@
         <v>2020</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F58" s="9">
         <v>44053</v>
@@ -22525,10 +22525,10 @@
         <v>3</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K58">
         <v>2</v>
@@ -22990,13 +22990,13 @@
         <v>1</v>
       </c>
       <c r="FL58" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM58" t="s">
         <v>249</v>
       </c>
-      <c r="FM58" t="s">
+      <c r="FN58" t="s">
         <v>250</v>
-      </c>
-      <c r="FN58" t="s">
-        <v>251</v>
       </c>
       <c r="FO58" s="1">
         <v>100</v>
@@ -23016,7 +23016,7 @@
     </row>
     <row r="60" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B60" s="3">
         <v>2020</v>
@@ -23025,10 +23025,10 @@
         <v>2020</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F60" s="9">
         <v>44053</v>
@@ -23040,10 +23040,10 @@
         <v>7</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K60">
         <v>2</v>
@@ -23505,13 +23505,13 @@
         <v>1</v>
       </c>
       <c r="FL60" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM60" t="s">
         <v>249</v>
       </c>
-      <c r="FM60" t="s">
+      <c r="FN60" t="s">
         <v>250</v>
-      </c>
-      <c r="FN60" t="s">
-        <v>251</v>
       </c>
       <c r="FO60" s="1">
         <v>100</v>
@@ -23519,7 +23519,7 @@
     </row>
     <row r="61" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B61" s="3">
         <v>2020</v>
@@ -23528,10 +23528,10 @@
         <v>2020</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F61" s="9">
         <v>44053</v>
@@ -23543,10 +23543,10 @@
         <v>8</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K61">
         <v>2</v>
@@ -24008,13 +24008,13 @@
         <v>1</v>
       </c>
       <c r="FL61" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM61" t="s">
         <v>249</v>
       </c>
-      <c r="FM61" t="s">
+      <c r="FN61" t="s">
         <v>250</v>
-      </c>
-      <c r="FN61" t="s">
-        <v>251</v>
       </c>
       <c r="FO61" s="1">
         <v>100</v>
@@ -24034,7 +24034,7 @@
     </row>
     <row r="63" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B63" s="3">
         <v>2020</v>
@@ -24043,10 +24043,10 @@
         <v>2020</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F63" s="9">
         <v>44087</v>
@@ -24058,10 +24058,10 @@
         <v>2</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K63">
         <v>1</v>
@@ -24523,13 +24523,13 @@
         <v>2</v>
       </c>
       <c r="FL63" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM63" t="s">
         <v>249</v>
       </c>
-      <c r="FM63" t="s">
+      <c r="FN63" t="s">
         <v>250</v>
-      </c>
-      <c r="FN63" t="s">
-        <v>251</v>
       </c>
       <c r="FO63" s="1">
         <v>100</v>
@@ -24537,7 +24537,7 @@
     </row>
     <row r="64" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B64" s="3">
         <v>2020</v>
@@ -24546,10 +24546,10 @@
         <v>2020</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F64" s="9">
         <v>44087</v>
@@ -24561,10 +24561,10 @@
         <v>3</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K64">
         <v>1</v>
@@ -25026,13 +25026,13 @@
         <v>2</v>
       </c>
       <c r="FL64" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM64" t="s">
         <v>249</v>
       </c>
-      <c r="FM64" t="s">
+      <c r="FN64" t="s">
         <v>250</v>
-      </c>
-      <c r="FN64" t="s">
-        <v>251</v>
       </c>
       <c r="FO64" s="1">
         <v>100</v>
@@ -25053,7 +25053,7 @@
     </row>
     <row r="66" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B66" s="3">
         <v>2020</v>
@@ -25062,10 +25062,10 @@
         <v>2020</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E66" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F66" s="9">
         <v>44087</v>
@@ -25077,10 +25077,10 @@
         <v>7</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K66">
         <v>1</v>
@@ -25542,13 +25542,13 @@
         <v>1</v>
       </c>
       <c r="FL66" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM66" t="s">
         <v>249</v>
       </c>
-      <c r="FM66" t="s">
+      <c r="FN66" t="s">
         <v>250</v>
-      </c>
-      <c r="FN66" t="s">
-        <v>251</v>
       </c>
       <c r="FO66" s="1">
         <v>100</v>
@@ -25556,7 +25556,7 @@
     </row>
     <row r="67" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B67" s="3">
         <v>2020</v>
@@ -25565,10 +25565,10 @@
         <v>2020</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F67" s="9">
         <v>44087</v>
@@ -25580,10 +25580,10 @@
         <v>8</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K67">
         <v>1</v>
@@ -26045,13 +26045,13 @@
         <v>1</v>
       </c>
       <c r="FL67" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM67" t="s">
         <v>249</v>
       </c>
-      <c r="FM67" t="s">
+      <c r="FN67" t="s">
         <v>250</v>
-      </c>
-      <c r="FN67" t="s">
-        <v>251</v>
       </c>
       <c r="FO67" s="1">
         <v>100</v>
@@ -26072,7 +26072,7 @@
     </row>
     <row r="69" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B69" s="3">
         <v>2020</v>
@@ -26081,10 +26081,10 @@
         <v>2020</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F69" s="9">
         <v>44087</v>
@@ -26096,10 +26096,10 @@
         <v>2</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K69">
         <v>2</v>
@@ -26561,13 +26561,13 @@
         <v>1</v>
       </c>
       <c r="FL69" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM69" t="s">
         <v>249</v>
       </c>
-      <c r="FM69" t="s">
+      <c r="FN69" t="s">
         <v>250</v>
-      </c>
-      <c r="FN69" t="s">
-        <v>251</v>
       </c>
       <c r="FO69" s="1">
         <v>100</v>
@@ -26575,7 +26575,7 @@
     </row>
     <row r="70" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B70" s="3">
         <v>2020</v>
@@ -26584,10 +26584,10 @@
         <v>2020</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E70" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F70" s="9">
         <v>44087</v>
@@ -26599,10 +26599,10 @@
         <v>3</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K70">
         <v>2</v>
@@ -27064,13 +27064,13 @@
         <v>1</v>
       </c>
       <c r="FL70" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM70" t="s">
         <v>249</v>
       </c>
-      <c r="FM70" t="s">
+      <c r="FN70" t="s">
         <v>250</v>
-      </c>
-      <c r="FN70" t="s">
-        <v>251</v>
       </c>
       <c r="FO70" s="1">
         <v>100</v>
@@ -27091,7 +27091,7 @@
     </row>
     <row r="72" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B72" s="3">
         <v>2020</v>
@@ -27100,10 +27100,10 @@
         <v>2020</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E72" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F72" s="9">
         <v>44087</v>
@@ -27115,10 +27115,10 @@
         <v>7</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K72">
         <v>2</v>
@@ -27580,13 +27580,13 @@
         <v>1</v>
       </c>
       <c r="FL72" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM72" t="s">
         <v>249</v>
       </c>
-      <c r="FM72" t="s">
+      <c r="FN72" t="s">
         <v>250</v>
-      </c>
-      <c r="FN72" t="s">
-        <v>251</v>
       </c>
       <c r="FO72" s="1">
         <v>100</v>
@@ -27594,7 +27594,7 @@
     </row>
     <row r="73" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B73" s="3">
         <v>2020</v>
@@ -27603,10 +27603,10 @@
         <v>2020</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F73" s="9">
         <v>44087</v>
@@ -27618,10 +27618,10 @@
         <v>8</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K73">
         <v>2</v>
@@ -28083,13 +28083,13 @@
         <v>1</v>
       </c>
       <c r="FL73" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM73" t="s">
         <v>249</v>
       </c>
-      <c r="FM73" t="s">
+      <c r="FN73" t="s">
         <v>250</v>
-      </c>
-      <c r="FN73" t="s">
-        <v>251</v>
       </c>
       <c r="FO73" s="1">
         <v>100</v>
@@ -28109,7 +28109,7 @@
     </row>
     <row r="75" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B75" s="3">
         <v>2020</v>
@@ -28118,10 +28118,10 @@
         <v>2020</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E75" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F75" s="9">
         <v>44110</v>
@@ -28133,10 +28133,10 @@
         <v>2</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K75">
         <v>1</v>
@@ -28598,13 +28598,13 @@
         <v>2</v>
       </c>
       <c r="FL75" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM75" t="s">
         <v>249</v>
       </c>
-      <c r="FM75" t="s">
+      <c r="FN75" t="s">
         <v>250</v>
-      </c>
-      <c r="FN75" t="s">
-        <v>251</v>
       </c>
       <c r="FO75" s="1">
         <v>100</v>
@@ -28612,7 +28612,7 @@
     </row>
     <row r="76" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B76" s="3">
         <v>2020</v>
@@ -28621,10 +28621,10 @@
         <v>2020</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E76" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F76" s="9">
         <v>44110</v>
@@ -28636,10 +28636,10 @@
         <v>3</v>
       </c>
       <c r="I76" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K76">
         <v>1</v>
@@ -29101,13 +29101,13 @@
         <v>1</v>
       </c>
       <c r="FL76" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM76" t="s">
         <v>249</v>
       </c>
-      <c r="FM76" t="s">
+      <c r="FN76" t="s">
         <v>250</v>
-      </c>
-      <c r="FN76" t="s">
-        <v>251</v>
       </c>
       <c r="FO76" s="1">
         <v>100</v>
@@ -29128,7 +29128,7 @@
     </row>
     <row r="78" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B78" s="3">
         <v>2020</v>
@@ -29137,10 +29137,10 @@
         <v>2020</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E78" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F78" s="9">
         <v>44110</v>
@@ -29152,10 +29152,10 @@
         <v>7</v>
       </c>
       <c r="I78" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K78">
         <v>1</v>
@@ -29617,13 +29617,13 @@
         <v>1</v>
       </c>
       <c r="FL78" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM78" t="s">
         <v>249</v>
       </c>
-      <c r="FM78" t="s">
+      <c r="FN78" t="s">
         <v>250</v>
-      </c>
-      <c r="FN78" t="s">
-        <v>251</v>
       </c>
       <c r="FO78" s="1">
         <v>100</v>
@@ -29631,7 +29631,7 @@
     </row>
     <row r="79" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B79" s="3">
         <v>2020</v>
@@ -29640,10 +29640,10 @@
         <v>2020</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E79" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F79" s="9">
         <v>44110</v>
@@ -29655,10 +29655,10 @@
         <v>8</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K79">
         <v>1</v>
@@ -30120,13 +30120,13 @@
         <v>1</v>
       </c>
       <c r="FL79" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM79" t="s">
         <v>249</v>
       </c>
-      <c r="FM79" t="s">
+      <c r="FN79" t="s">
         <v>250</v>
-      </c>
-      <c r="FN79" t="s">
-        <v>251</v>
       </c>
       <c r="FO79" s="1">
         <v>100</v>
@@ -30147,7 +30147,7 @@
     </row>
     <row r="81" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B81" s="3">
         <v>2020</v>
@@ -30156,10 +30156,10 @@
         <v>2020</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E81" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F81" s="9">
         <v>44110</v>
@@ -30171,10 +30171,10 @@
         <v>2</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K81">
         <v>2</v>
@@ -30636,13 +30636,13 @@
         <v>1</v>
       </c>
       <c r="FL81" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM81" t="s">
         <v>249</v>
       </c>
-      <c r="FM81" t="s">
+      <c r="FN81" t="s">
         <v>250</v>
-      </c>
-      <c r="FN81" t="s">
-        <v>251</v>
       </c>
       <c r="FO81" s="1">
         <v>100</v>
@@ -30650,7 +30650,7 @@
     </row>
     <row r="82" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B82" s="3">
         <v>2020</v>
@@ -30659,10 +30659,10 @@
         <v>2020</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F82" s="9">
         <v>44110</v>
@@ -30674,10 +30674,10 @@
         <v>3</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K82">
         <v>2</v>
@@ -31139,13 +31139,13 @@
         <v>2</v>
       </c>
       <c r="FL82" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM82" t="s">
         <v>249</v>
       </c>
-      <c r="FM82" t="s">
+      <c r="FN82" t="s">
         <v>250</v>
-      </c>
-      <c r="FN82" t="s">
-        <v>251</v>
       </c>
       <c r="FO82" s="1">
         <v>100</v>
@@ -31166,7 +31166,7 @@
     </row>
     <row r="84" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B84" s="3">
         <v>2020</v>
@@ -31175,10 +31175,10 @@
         <v>2020</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E84" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F84" s="9">
         <v>44110</v>
@@ -31190,10 +31190,10 @@
         <v>7</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K84">
         <v>2</v>
@@ -31655,13 +31655,13 @@
         <v>1</v>
       </c>
       <c r="FL84" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM84" t="s">
         <v>249</v>
       </c>
-      <c r="FM84" t="s">
+      <c r="FN84" t="s">
         <v>250</v>
-      </c>
-      <c r="FN84" t="s">
-        <v>251</v>
       </c>
       <c r="FO84" s="1">
         <v>100</v>
@@ -31669,7 +31669,7 @@
     </row>
     <row r="85" spans="1:171" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B85" s="3">
         <v>2020</v>
@@ -31678,10 +31678,10 @@
         <v>2020</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E85" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F85" s="9">
         <v>44110</v>
@@ -31693,10 +31693,10 @@
         <v>8</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K85">
         <v>2</v>
@@ -32158,13 +32158,13 @@
         <v>2</v>
       </c>
       <c r="FL85" t="s">
+        <v>248</v>
+      </c>
+      <c r="FM85" t="s">
         <v>249</v>
       </c>
-      <c r="FM85" t="s">
+      <c r="FN85" t="s">
         <v>250</v>
-      </c>
-      <c r="FN85" t="s">
-        <v>251</v>
       </c>
       <c r="FO85" s="1">
         <v>100</v>

</xml_diff>